<commit_message>
before ubuntu git clone
</commit_message>
<xml_diff>
--- a/transactions2.xlsx
+++ b/transactions2.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <plotArea>
       <barChart>
@@ -159,7 +159,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -173,7 +173,7 @@
           <idx val="1"/>
           <order val="1"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>5</col>
@@ -235,9 +235,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -530,7 +530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
@@ -625,6 +625,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>